<commit_message>
modify ClimaWatch Testing Documentation.xlsx
</commit_message>
<xml_diff>
--- a/ClimaWatch Testing Documentation.xlsx
+++ b/ClimaWatch Testing Documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41fb85a9a0361d73/Desktop/ClimaWatch Testing Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Super\Revature\Project 2\BKDS\ClimaWatch Testing Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B116059-2D1F-464C-BABA-641894635096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D52227-BEE7-4E52-9DED-7696189FD261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2340" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="5" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="8" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="CWL-Test Scenario" sheetId="4" r:id="rId5"/>
     <sheet name="CWH-Test Cases" sheetId="6" r:id="rId6"/>
     <sheet name="CWR-Test Cases" sheetId="7" r:id="rId7"/>
+    <sheet name="CWL-Test Cases" sheetId="8" r:id="rId8"/>
+    <sheet name="RequirementsTraceability Matrix" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -487,22 +489,118 @@
     <t>CWRTC-14</t>
   </si>
   <si>
-    <t>Register for an account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Put URI in the web browser
- = http://127.0.0.1:5501
-Click Join Now </t>
-  </si>
-  <si>
-    <t>Registration form appears</t>
-  </si>
-  <si>
-    <t>Register with vaild credentials</t>
+    <t>CWLTC-1</t>
+  </si>
+  <si>
+    <t>CWLTC-2</t>
+  </si>
+  <si>
+    <t>CWLTC-3</t>
+  </si>
+  <si>
+    <t>CWLTC-4</t>
+  </si>
+  <si>
+    <t>CWLTC-5</t>
+  </si>
+  <si>
+    <t>CWLTC-6</t>
+  </si>
+  <si>
+    <t>CWLTC-7</t>
+  </si>
+  <si>
+    <t>CWLTC-8</t>
   </si>
   <si>
     <t>1. Open site
-2. Click on join now</t>
+2. Click on sign in
+3. Input blank username
+4. Input vaild password</t>
+  </si>
+  <si>
+    <t>Username = &lt;blank&gt;
+password = password
+Click sign in button</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on sign in
+3. Input vaild username
+4. Input vaild password</t>
+  </si>
+  <si>
+    <t>Username = bipul513
+password = password
+Click sign in button</t>
+  </si>
+  <si>
+    <t>Page refreshes with user favorite weather forecasts and current news</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on sign in
+3. Input vaild username
+4. Input blank password</t>
+  </si>
+  <si>
+    <t>Username = bipul513
+password = &lt;blank&gt;
+Click sign in button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on sign in
+3. Input invaild username
+4. Input vaild password</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on sign in
+3. Input vaild username
+4. Input invaild password</t>
+  </si>
+  <si>
+    <t>Username = kratos12
+password = password
+Click sign in button</t>
+  </si>
+  <si>
+    <t>Username = bipul513
+password = abc123
+Click sign in button</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input blank username
+4. Input vaild name
+5. Input vaild email
+6. Input vaild password
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = &lt;blank&gt;
+Name = Freya
+Email = freya18@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Username = freya11
+Name = Freya
+Email = freya18@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Registration success message</t>
   </si>
   <si>
     <t>1. Open site
@@ -514,50 +612,194 @@
 7. Click join now button</t>
   </si>
   <si>
-    <t>Username = ryan17
-Name = Ryan
-Email = ryan17@abc.com
-password = password
-Click join now button</t>
-  </si>
-  <si>
-    <t>Registration successfully message</t>
-  </si>
-  <si>
     <t>1. Open site
 2. Click on join now
-3. Input blank username
+3. Username already exists
 4. Input vaild name
 5. Input vaild email
 6. Input vaild password
 7. Click join now button</t>
   </si>
   <si>
-    <t>Username = &lt;blank&gt;
-Name = Freya
-Email = freya18@abc.com
+    <t>Username = freya11
+Name = Odin
+Email = ninerelams@abc.com
 password = password
 Click join now button</t>
   </si>
   <si>
-    <t xml:space="preserve">Error message </t>
-  </si>
-  <si>
-    <t>Username already exists</t>
-  </si>
-  <si>
     <t>1. Open site
 2. Click on join now
-3. Input username that exists already
+3. Username does not already exist
 4. Input vaild name
 5. Input vaild email
 6. Input vaild password
 7. Click join now button</t>
   </si>
   <si>
-    <t>Username = ryan17
-Name = Freya
-Email = freya18@abc.com
+    <t>Username = raven11
+Name = Odin
+Email = ninerelams@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Username = thor12
+Name = Thor
+Email = thorhammer12@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Username = thor12
+Name = Thor
+Email = thorhammer12@abc.com
+password = &lt;blank&gt;
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input vaild name
+5. Input vaild email
+6. Input password is blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input vaild name
+5. Input vaild email
+6. Input password is not blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input name with special characters/number
+5. Input vaild email
+6. Input password is not blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = loki8
+Name = L@k1
+Email = icegiantjoker@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input name has alphabetical characters only
+5. Input vaild email
+6. Input password is not blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = loki8
+Name = Loki
+Email = icegiantjoker@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input name has alphabetical characters only
+5. Input email is blank
+6. Input password is not blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = heimdall9
+Name = Heimdall
+Email = &lt;blank&gt;
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Username = heimdall9
+Name = Heimdall
+Email = gates09@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input vaild name
+5. Input email is not blank
+6. Input password is not blank
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = modi2
+Name = Modi
+Email = thorhammer12@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>Username = tyr4
+Name = Tyr
+Email = wargod4#abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input valid name
+5. Input email does not have correct format
+6. Input vaild password
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input valid name
+5. Input email has correct format
+6. Input valid password
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = tyr4
+Name = Tyr
+Email = wargod4@abc.com
+password = password
+Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input valid name
+5. Input email already used by another user
+6. Input valid password
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Click on join now
+3. Input vaild username
+4. Input valid name
+5. Input email is not already used by another user
+6. Input valid password
+7. Click join now button</t>
+  </si>
+  <si>
+    <t>Username = modi2
+Name = Modi
+Email = secondson@abc.com
 password = password
 Click join now button</t>
   </si>
@@ -938,7 +1180,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1440,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1287,7 +1529,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1486,7 +1728,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="A1:F10"/>
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1B2EC0-0381-4C6E-8442-6145589D1A82}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1749,26 +1991,26 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421EF579-D24F-4850-8074-B601D5936424}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="29.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
+    <col min="3" max="3" width="44.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1779,6 +2021,310 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E16" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23936664-8419-47B4-B92A-116E859C9A39}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" customWidth="1"/>
+    <col min="5" max="5" width="57.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1803,125 +2349,140 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>146</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>133</v>
-      </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" t="s">
         <v>158</v>
       </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>144</v>
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1931,4 +2492,321 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443060C-FCED-4446-959C-A1656DDF5BBC}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify ClimaWatch Testing Documentation and add ClimaWatch Defect Report.xlsx
</commit_message>
<xml_diff>
--- a/ClimaWatch Testing Documentation.xlsx
+++ b/ClimaWatch Testing Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Super\Revature\Project 2\BKDS\ClimaWatch Testing Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D52227-BEE7-4E52-9DED-7696189FD261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9055535-D21A-4180-BD17-43CD70AC2E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="8" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,12 @@
     <sheet name="CWH-Test Scenario" sheetId="5" r:id="rId3"/>
     <sheet name="CWR-Test Scenario" sheetId="3" r:id="rId4"/>
     <sheet name="CWL-Test Scenario" sheetId="4" r:id="rId5"/>
-    <sheet name="CWH-Test Cases" sheetId="6" r:id="rId6"/>
-    <sheet name="CWR-Test Cases" sheetId="7" r:id="rId7"/>
-    <sheet name="CWL-Test Cases" sheetId="8" r:id="rId8"/>
-    <sheet name="RequirementsTraceability Matrix" sheetId="9" r:id="rId9"/>
+    <sheet name="CWF-Test Scenario" sheetId="10" r:id="rId6"/>
+    <sheet name="CWH-Test Cases" sheetId="6" r:id="rId7"/>
+    <sheet name="CWR-Test Cases" sheetId="7" r:id="rId8"/>
+    <sheet name="CWL-Test Cases" sheetId="8" r:id="rId9"/>
+    <sheet name="CWF-Test Cases" sheetId="11" r:id="rId10"/>
+    <sheet name="RequirementsTraceability Matrix" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="222">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -390,10 +392,6 @@
 2. Pay attention to page layout</t>
   </si>
   <si>
-    <t>Put URI in the web browser
- = http://127.0.0.1:5501</t>
-  </si>
-  <si>
     <t>Check homepage does not display</t>
   </si>
   <si>
@@ -401,10 +399,6 @@
 2. Pay attention to page </t>
   </si>
   <si>
-    <t>Put URI in the web browser
- = http://127.0.0.2:5501</t>
-  </si>
-  <si>
     <t>Hompage is not opened</t>
   </si>
   <si>
@@ -425,9 +419,6 @@
   </si>
   <si>
     <t>Click Search</t>
-  </si>
-  <si>
-    <t>"City not found!!"</t>
   </si>
   <si>
     <t>CWHTC-4</t>
@@ -802,6 +793,100 @@
 Email = secondson@abc.com
 password = password
 Click join now button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hompage Opens </t>
+  </si>
+  <si>
+    <t>Put URI in the web browser
+ = http://127.0.0.1:5501/index.html</t>
+  </si>
+  <si>
+    <t>Put URI in the web browser
+ = http://127.0.0.2:5500/index.html</t>
+  </si>
+  <si>
+    <t>Display message: "This site can't be reached"</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>"City not found !!!"</t>
+  </si>
+  <si>
+    <t>Display message: "City not found !!!"</t>
+  </si>
+  <si>
+    <t>Current weather for Rome, IT is displayed</t>
+  </si>
+  <si>
+    <t>"Please sign in with valid credentials"</t>
+  </si>
+  <si>
+    <t>Display: "Please sign in with valid credentials"</t>
+  </si>
+  <si>
+    <t>Please enter all the details in the correct format!!!</t>
+  </si>
+  <si>
+    <t>Display:"Freya Welcome to ClimaWatch!!! Please sign in using your username and explore additional features of ClimaWatch !!!"</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>M-4</t>
+  </si>
+  <si>
+    <t>Favorite Locations</t>
+  </si>
+  <si>
+    <t>CWF-1</t>
+  </si>
+  <si>
+    <t>CWF-2</t>
+  </si>
+  <si>
+    <t>CWF-3</t>
+  </si>
+  <si>
+    <t>Add to Favorites button must be clicked</t>
+  </si>
+  <si>
+    <t>Removed Favorites button must be clicked</t>
+  </si>
+  <si>
+    <t>CWFT-1</t>
+  </si>
+  <si>
+    <t>CWFT-2</t>
+  </si>
+  <si>
+    <t>CWFT-3</t>
+  </si>
+  <si>
+    <t>CWFT-4</t>
+  </si>
+  <si>
+    <t>Location search bar is not blank</t>
+  </si>
+  <si>
+    <t>Add to Favorite button is clicked</t>
+  </si>
+  <si>
+    <t>Remove Favorite button is clicked</t>
+  </si>
+  <si>
+    <t>Check Add to Favorites button adds Favorite</t>
+  </si>
+  <si>
+    <t>Check Remove Favorite button remove Favorite</t>
+  </si>
+  <si>
+    <t>1. Open site
+2. Login with vaild credentals
+2. Pay attention to page layout</t>
   </si>
 </sst>
 </file>
@@ -1177,16 +1262,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F298C-ABAA-4CB8-A732-AC0F2DDD5EC1}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="47.109375" customWidth="1"/>
   </cols>
@@ -1335,7 +1420,511 @@
         <v>29</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF823818-5B3A-475B-919B-7768B09AD044}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="46.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443060C-FCED-4446-959C-A1656DDF5BBC}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1344,7 +1933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDE58C-1172-4D53-B894-2331B214C78C}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1440,7 +2029,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1452,7 +2041,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1857,11 +2446,99 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AF602B8-74EA-4575-9CC8-D5768BD330E7}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1B2EC0-0381-4C6E-8442-6145589D1A82}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K2"/>
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,9 +2546,9 @@
     <col min="1" max="1" width="10.44140625" customWidth="1"/>
     <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="3" max="3" width="35.21875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1913,7 +2590,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -1924,61 +2601,85 @@
         <v>113</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>114</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E4" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>118</v>
+      <c r="F4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" t="s">
-        <v>124</v>
-      </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>197</v>
+      </c>
+      <c r="F5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
         <v>126</v>
       </c>
-      <c r="B6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" t="s">
-        <v>129</v>
+      <c r="F6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1989,12 +2690,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421EF579-D24F-4850-8074-B601D5936424}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="E1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2003,8 +2704,8 @@
     <col min="2" max="2" width="45.21875" customWidth="1"/>
     <col min="3" max="3" width="44.88671875" customWidth="1"/>
     <col min="4" max="4" width="34.21875" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" customWidth="1"/>
+    <col min="6" max="6" width="109.88671875" customWidth="1"/>
     <col min="7" max="7" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2048,240 +2749,246 @@
     </row>
     <row r="3" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>202</v>
+      </c>
+      <c r="F3" t="s">
+        <v>203</v>
+      </c>
+      <c r="G3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
         <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
         <v>74</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
         <v>78</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2293,12 +3000,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23936664-8419-47B4-B92A-116E859C9A39}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2307,8 +3014,7 @@
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="28.77734375" customWidth="1"/>
     <col min="4" max="4" width="32.109375" customWidth="1"/>
-    <col min="5" max="5" width="57.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="5" max="6" width="57.44140625" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2351,138 +3057,186 @@
     </row>
     <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>200</v>
+      </c>
+      <c r="F3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="F4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>200</v>
+      </c>
+      <c r="F5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="F6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
         <v>90</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="F8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G8" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
         <v>91</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>200</v>
+      </c>
+      <c r="F9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2492,321 +3246,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443060C-FCED-4446-959C-A1656DDF5BBC}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="3" width="17.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" t="s">
-        <v>145</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" t="s">
-        <v>148</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>150</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" t="s">
-        <v>152</v>
-      </c>
-      <c r="C27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modify ClimaWatch Testing Documention.xlsx
</commit_message>
<xml_diff>
--- a/ClimaWatch Testing Documentation.xlsx
+++ b/ClimaWatch Testing Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Super\Revature\Project 2\BKDS\ClimaWatch Testing Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0950A7B-CF92-4116-8144-FA30E07C4AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164529F2-0A13-49D8-80DF-C27293216479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{8A1B809B-9824-45A6-9207-C365FE3942EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="226">
   <si>
     <t xml:space="preserve">User Story </t>
   </si>
@@ -889,6 +889,18 @@
   </si>
   <si>
     <t>ClimaWatch: Requirements Traceability Matrix</t>
+  </si>
+  <si>
+    <t>CWFTC-1</t>
+  </si>
+  <si>
+    <t>CWFTC-2</t>
+  </si>
+  <si>
+    <t>CWFTC-3</t>
+  </si>
+  <si>
+    <t>CWFTC-4</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40F298C-ABAA-4CB8-A732-AC0F2DDD5EC1}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -1460,7 +1472,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,7 +1525,7 @@
     </row>
     <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
         <v>105</v>
@@ -1536,7 +1548,7 @@
     </row>
     <row r="4" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
         <v>109</v>
@@ -1559,7 +1571,7 @@
     </row>
     <row r="5" spans="1:11" ht="103.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="B5" t="s">
         <v>184</v>
@@ -1582,7 +1594,7 @@
     </row>
     <row r="6" spans="1:11" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
         <v>185</v>
@@ -1607,6 +1619,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1615,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5443060C-FCED-4446-959C-A1656DDF5BBC}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,10 +1709,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -1707,10 +1720,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -1718,10 +1731,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
@@ -1729,10 +1742,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
@@ -1740,10 +1753,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>117</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
@@ -1751,10 +1764,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>118</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -1762,10 +1775,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
       </c>
       <c r="C13" t="s">
         <v>36</v>
@@ -1773,10 +1786,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
@@ -1784,10 +1797,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
-      </c>
-      <c r="B15" t="s">
-        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -1795,10 +1808,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
         <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -1806,10 +1819,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
         <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>123</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1817,10 +1830,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1828,10 +1841,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
         <v>69</v>
-      </c>
-      <c r="B19" t="s">
-        <v>125</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -1839,10 +1852,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
         <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>126</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -1850,10 +1863,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>127</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
@@ -1861,10 +1874,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
         <v>72</v>
-      </c>
-      <c r="B22" t="s">
-        <v>128</v>
       </c>
       <c r="C22" t="s">
         <v>40</v>
@@ -1872,10 +1885,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
         <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -1883,10 +1896,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
         <v>74</v>
-      </c>
-      <c r="B24" t="s">
-        <v>130</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -2378,7 +2391,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2449,7 +2462,7 @@
         <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>